<commit_message>
fix(solver): Handles tables in range variables
</commit_message>
<xml_diff>
--- a/examples/checker.xlsx
+++ b/examples/checker.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Mark\Projects\ExCell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Mark\dev\ExCell\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="2" r:id="rId1"/>
@@ -21,14 +21,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tony Rogers</author>
     <author>Mark</author>
     <author>Mark Fairhurst</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="1" shapeId="0">
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -141,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="2" shapeId="0">
+    <comment ref="B22" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -189,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B23" authorId="2" shapeId="0">
+    <comment ref="B23" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -213,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="2" shapeId="0">
+    <comment ref="B24" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B25" authorId="2" shapeId="0">
+    <comment ref="B25" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +438,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,10 +620,10 @@
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Percent 2" xfId="2"/>
-    <cellStyle name="Percent 3" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Percent 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -958,7 +958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -1135,12 +1135,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,12 +1172,6 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
       <c r="J2" t="s">
         <v>8</v>
       </c>
@@ -1196,6 +1190,9 @@
         <v>27</v>
       </c>
       <c r="B3" s="9"/>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="G3">
         <v>0</v>
       </c>
@@ -1218,7 +1215,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f>IF(B4&gt;0,10,0)</f>
+        <f t="shared" ref="C4:C13" si="0">IF(B4&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F4">
@@ -1237,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(B5&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5">
@@ -1256,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(B6&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6">
@@ -1278,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(B7&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7">
@@ -1297,7 +1294,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(B8&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8">
@@ -1316,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(B9&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9">
@@ -1335,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(B10&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10">
@@ -1354,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(B11&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11">
@@ -1373,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(B12&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F12">
@@ -1392,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(B13&gt;0,10,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13">
@@ -1410,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>VLOOKUP(B14,F2:G13,2)</f>
+        <f>VLOOKUP(B14,F3:G13,2)</f>
         <v>0</v>
       </c>
     </row>
@@ -1489,7 +1486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B16"/>
   <sheetViews>

</xml_diff>